<commit_message>
added scraper for NF group for St. Petersburg
</commit_message>
<xml_diff>
--- a/commerce_estate/Etagi/data/Sales.xlsx
+++ b/commerce_estate/Etagi/data/Sales.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1129,6 +1129,94 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>10056376</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://spb.etagi.com/realty/10056376</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>offices</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>office</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург город, Центральный район, Старорусская улица, 5к.3</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Санкт Петербург</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>59.932626</v>
+      </c>
+      <c r="I9" t="n">
+        <v>30.384311</v>
+      </c>
+      <c r="J9" t="n">
+        <v>16500000</v>
+      </c>
+      <c r="K9" t="n">
+        <v>171875</v>
+      </c>
+      <c r="L9" t="n">
+        <v>96</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>23_10_2023</t>
+        </is>
+      </c>
+      <c r="N9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Площадь Александра Невского - 1</t>
+        </is>
+      </c>
+      <c r="P9" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="n">
+        <v>1</v>
+      </c>
+      <c r="S9" t="n">
+        <v>6</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>living</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>https://cdn.esoft.digital/19201080/cluster/photos/64/82/949abfe91827b638223aaa1a36005f513d608264.jpeg</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>25/10/2023</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>